<commit_message>
RO: emporium methods and update mainwin to pair serving to customers
</commit_message>
<xml_diff>
--- a/P11/Scrum_MICE_Sprint_5.xlsx
+++ b/P11/Scrum_MICE_Sprint_5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haydenjohnson/Code/cse1325/P11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E270DF-B6B3-E342-88A3-CDA0C8916834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46E904A-1A7F-B74C-B304-A609C9AF8E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="213">
   <si>
     <t>Product Name:</t>
   </si>
@@ -653,9 +653,6 @@
     <t>Finished in Sprint 4</t>
   </si>
   <si>
-    <t>In Work</t>
-  </si>
-  <si>
     <t>Blue Bumpkins</t>
   </si>
   <si>
@@ -663,6 +660,27 @@
   </si>
   <si>
     <t>HJ</t>
+  </si>
+  <si>
+    <t>Compile and test price and cost methods, update view to display Order summary.</t>
+  </si>
+  <si>
+    <t>Finished in Sprint 5</t>
+  </si>
+  <si>
+    <t>Completed Day 7</t>
+  </si>
+  <si>
+    <t>Compile and test methods for customers, implement favorite customer</t>
+  </si>
+  <si>
+    <t>Add feature to limit max scoops, compile, and test</t>
+  </si>
+  <si>
+    <t>Add necessary methods to Emporium to match servings with customer, update onCreateServing method, compile, test</t>
+  </si>
+  <si>
+    <t>Add customer object to order class, compile and test</t>
   </si>
 </sst>
 </file>
@@ -674,7 +692,7 @@
     <numFmt numFmtId="165" formatCode="mmm\ dd"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -758,6 +776,12 @@
       <name val="Arial"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -822,7 +846,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -915,6 +939,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1152,10 +1177,10 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2691,28 +2716,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2927,7 +2952,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -3075,7 +3100,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -3149,7 +3174,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -3810,8 +3835,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="A30" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -3853,7 +3878,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C2" s="35"/>
       <c r="D2" s="35"/>
@@ -3899,7 +3924,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
@@ -3907,7 +3932,7 @@
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>
       <c r="H5" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I5" s="2">
         <v>1001871835</v>
@@ -4113,11 +4138,11 @@
       </c>
       <c r="B17" s="4">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C17" s="8">
         <f>COUNTIF(G$24:G$110,"Finished in Sprint 5")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="4"/>
@@ -4133,7 +4158,7 @@
       </c>
       <c r="B18" s="4">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C18" s="8">
         <f>COUNTIF(G$24:G$110,"Finished in Sprint 6")</f>
@@ -4708,7 +4733,7 @@
         <v>5</v>
       </c>
       <c r="G38" s="14" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="H38" s="31" t="s">
         <v>31</v>
@@ -4741,7 +4766,7 @@
         <v>5</v>
       </c>
       <c r="G39" s="14" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="H39" s="31" t="s">
         <v>54</v>
@@ -4774,7 +4799,7 @@
         <v>5</v>
       </c>
       <c r="G40" s="14" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="H40" s="31" t="s">
         <v>74</v>
@@ -4807,7 +4832,7 @@
         <v>5</v>
       </c>
       <c r="G41" s="14" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="H41" s="31" t="s">
         <v>31</v>
@@ -4838,7 +4863,7 @@
         <v>5</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="H42" s="31" t="s">
         <v>54</v>
@@ -5959,7 +5984,7 @@
       <formula1>"1,2,3,4,5,6"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Status" prompt="Leave blank initially (hint: Use the Delete key)_x000a_Select &quot;In Work&quot; when you begin designing and coding this feature._x000a_Select &quot;In Test&quot; when this feature is fully coded and you are testing it._x000a_Select  Finished ONLY when the feature works well and is READY TO" sqref="G24:G42 G69:G104" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Status" prompt="Leave blank initially (hint: Use the Delete key)_x000a_Select &quot;In Work&quot; when you begin designing and coding this feature._x000a_Select &quot;In Test&quot; when this feature is fully coded and you are testing it._x000a_Select  Finished ONLY when the feature works well and is READY TO" sqref="G69:G104 G24:G42" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>"In Work,In Test,Finished in Sprint 1,Finished in Sprint 2,Finished in Sprint 3,Finished in Sprint 4,Finished in Sprint 5,Finished in Sprint 6"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9982,8 +10007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -10088,7 +10113,7 @@
       </c>
       <c r="B7" s="18">
         <f>COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -10103,7 +10128,7 @@
       </c>
       <c r="B8" s="18">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C8" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -10121,7 +10146,7 @@
       </c>
       <c r="B9" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C9" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -10139,7 +10164,7 @@
       </c>
       <c r="B10" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C10" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -10157,7 +10182,7 @@
       </c>
       <c r="B11" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C11" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -10175,7 +10200,7 @@
       </c>
       <c r="B12" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C12" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -10193,7 +10218,7 @@
       </c>
       <c r="B13" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C13" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -10211,11 +10236,11 @@
       </c>
       <c r="B14" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
@@ -10260,10 +10285,15 @@
       <c r="B17" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="27" t="s">
-        <v>196</v>
-      </c>
-      <c r="E17" s="28"/>
+      <c r="C17" t="s">
+        <v>205</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>210</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
@@ -10272,8 +10302,15 @@
       <c r="B18" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="28"/>
+      <c r="C18" t="s">
+        <v>205</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
@@ -10282,8 +10319,15 @@
       <c r="B19" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="28"/>
+      <c r="C19" t="s">
+        <v>205</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
@@ -10292,8 +10336,15 @@
       <c r="B20" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="28"/>
+      <c r="C20" t="s">
+        <v>205</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
@@ -10302,8 +10353,15 @@
       <c r="B21" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="28"/>
+      <c r="C21" t="s">
+        <v>205</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">

</xml_diff>